<commit_message>
Added new feature / Updated files
</commit_message>
<xml_diff>
--- a/backend/Childsurvey.xlsx
+++ b/backend/Childsurvey.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W522"/>
+  <dimension ref="A1:W523"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32637,6 +32637,63 @@
       <c r="V522" t="inlineStr"/>
       <c r="W522" t="inlineStr"/>
     </row>
+    <row r="523">
+      <c r="A523" t="inlineStr"/>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Yogesh Mittal</t>
+        </is>
+      </c>
+      <c r="C523" t="n">
+        <v>7</v>
+      </c>
+      <c r="D523" t="inlineStr"/>
+      <c r="E523" t="n">
+        <v>5</v>
+      </c>
+      <c r="F523" t="inlineStr">
+        <is>
+          <t>Private Job</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Financial </t>
+        </is>
+      </c>
+      <c r="H523" t="inlineStr">
+        <is>
+          <t>No effect</t>
+        </is>
+      </c>
+      <c r="I523" t="n">
+        <v>7</v>
+      </c>
+      <c r="J523" t="n">
+        <v>40000</v>
+      </c>
+      <c r="K523" t="inlineStr">
+        <is>
+          <t>Army</t>
+        </is>
+      </c>
+      <c r="L523" t="inlineStr">
+        <is>
+          <t>Loves army</t>
+        </is>
+      </c>
+      <c r="M523" t="inlineStr"/>
+      <c r="N523" t="inlineStr"/>
+      <c r="O523" t="inlineStr"/>
+      <c r="P523" t="inlineStr"/>
+      <c r="Q523" t="inlineStr"/>
+      <c r="R523" t="inlineStr"/>
+      <c r="S523" t="inlineStr"/>
+      <c r="T523" t="inlineStr"/>
+      <c r="U523" t="inlineStr"/>
+      <c r="V523" t="inlineStr"/>
+      <c r="W523" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>